<commit_message>
Bleed Status + bleed and poison animation. Equipment test and equipment change in battle test. Inventory Equipment Stack logic changed
</commit_message>
<xml_diff>
--- a/documentation/Items.xlsx
+++ b/documentation/Items.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheqs\Desktop\Hus 'n' Hus Game Studio\DRogue Lite\DRoque-Lite\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46293398-AB33-42CB-868B-2AB00693B6F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15E370A9-C0C4-4CF4-B7A6-7DF5A3526CC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
   <si>
     <t>ID</t>
   </si>
@@ -67,13 +67,58 @@
   </si>
   <si>
     <t>USABLE</t>
+  </si>
+  <si>
+    <t>BasicShirt</t>
+  </si>
+  <si>
+    <t>Zucchetto</t>
+  </si>
+  <si>
+    <t>Torch</t>
+  </si>
+  <si>
+    <t>ARMOR</t>
+  </si>
+  <si>
+    <t>vit, maxHealth</t>
+  </si>
+  <si>
+    <t>int, wis, maxMana</t>
+  </si>
+  <si>
+    <t>OFFHAND</t>
+  </si>
+  <si>
+    <t>agi, dex</t>
+  </si>
+  <si>
+    <t>BasicShield</t>
+  </si>
+  <si>
+    <t>vit, vit, vit, maxHealth</t>
+  </si>
+  <si>
+    <t>IronNecklace</t>
+  </si>
+  <si>
+    <t>Accessory</t>
+  </si>
+  <si>
+    <t>int, agi</t>
+  </si>
+  <si>
+    <t>RubyRing</t>
+  </si>
+  <si>
+    <t>str, wis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,14 +151,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -189,10 +226,10 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -481,7 +518,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,7 +526,8 @@
     <col min="1" max="1" width="9.140625" style="7"/>
     <col min="2" max="2" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -561,6 +599,108 @@
         <v>12</v>
       </c>
     </row>
+    <row r="5" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>8</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E12" s="3"/>
     </row>

</xml_diff>

<commit_message>
Learn skill in battle + skill replacement
</commit_message>
<xml_diff>
--- a/documentation/Items.xlsx
+++ b/documentation/Items.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheqs\Desktop\Hus 'n' Hus Game Studio\DRogue Lite\DRoque-Lite\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C872B3B-128C-4DE9-B6C1-155ED8FE7433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{561FD29C-74FE-49BE-9378-5F366B61F398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
   <si>
     <t>ID</t>
   </si>
@@ -115,13 +115,16 @@
   </si>
   <si>
     <t>UpgradeI</t>
+  </si>
+  <si>
+    <t>SkillLearner</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,14 +149,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -206,15 +201,12 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
@@ -515,12 +507,12 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="7"/>
+    <col min="1" max="1" width="9.140625" style="6"/>
     <col min="2" max="2" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -529,7 +521,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -545,178 +537,192 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+    <row r="2" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+    <row r="3" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="4" t="s">
+      <c r="D3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+    <row r="4" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="4" t="s">
+      <c r="D4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+    <row r="5" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
         <v>3</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="4" t="s">
+      <c r="D5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+    <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="4" t="s">
+      <c r="D6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
+    <row r="7" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
         <v>5</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="4" t="s">
+      <c r="D7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
+    <row r="8" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
         <v>6</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="4" t="s">
+      <c r="D8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
+    <row r="9" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
         <v>7</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="4" t="s">
+      <c r="D9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
+    <row r="10" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
         <v>8</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="4" t="s">
+      <c r="D10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
-        <v>9</v>
-      </c>
-      <c r="B11" s="4" t="s">
+    <row r="11" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E12" s="3"/>
+    <row r="12" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fusion Evolution System + Some bug fixes (a large number to be listed Lol)
</commit_message>
<xml_diff>
--- a/documentation/Items.xlsx
+++ b/documentation/Items.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheqs\Desktop\Hus 'n' Hus Game Studio\DRogue Lite\DRoque-Lite\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{561FD29C-74FE-49BE-9378-5F366B61F398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D059B58A-187D-40AE-8EF7-824A881D5CAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="32">
   <si>
     <t>ID</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>SkillLearner</t>
+  </si>
+  <si>
+    <t>UniqueDNA</t>
   </si>
 </sst>
 </file>
@@ -504,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -724,6 +727,23 @@
         <v>10</v>
       </c>
     </row>
+    <row r="13" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>